<commit_message>
tempi presi per elab2 openMp
</commit_message>
<xml_diff>
--- a/elaborati_open_mp/elaborato_2/test_valutazione_elab2_OpenMp.xlsx
+++ b/elaborati_open_mp/elaborato_2/test_valutazione_elab2_OpenMp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa0l0\Documents\GitHub\Calcolo-Parallelo\elaborati_open_mp\elaborato_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225AB62E-B6AD-49BE-AB62-6ACE706EA07A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC7BAE1-939F-4CBC-A620-6E0CF4207933}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>CALCOLO SPEEDUP</t>
   </si>
@@ -71,6 +71,52 @@
   <si>
     <t>M&lt;N, M=1000</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vengono tempi in maggioranza peggiori del caso M&gt;N tranne </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>questi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> !!!!! </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nel caso quadrato escono </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>tempi poco coerenti</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> !!!!!</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -96,18 +142,18 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -120,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -255,11 +301,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -318,7 +432,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -331,46 +444,56 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -687,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -837,16 +960,16 @@
         <v>2</v>
       </c>
       <c r="C5" s="12">
-        <f>C$68/C47</f>
-        <v>1.6511837547449049</v>
+        <f t="shared" ref="C5:E7" si="0">C$68/C47</f>
+        <v>1.4854810237332494</v>
       </c>
       <c r="D5" s="12">
-        <f>D$68/D47</f>
-        <v>1.3522242914820484</v>
+        <f t="shared" si="0"/>
+        <v>1.9439536024929378</v>
       </c>
       <c r="E5" s="13">
-        <f>E$68/E47</f>
-        <v>1.1232421554088814</v>
+        <f t="shared" si="0"/>
+        <v>1.9911291403340701</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -876,16 +999,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="12">
-        <f>C$68/C48</f>
-        <v>3.2756656910388093</v>
+        <f t="shared" si="0"/>
+        <v>2.6392504292042069</v>
       </c>
       <c r="D6" s="12">
-        <f>D$68/D48</f>
-        <v>3.3101274182932832</v>
+        <f t="shared" si="0"/>
+        <v>3.5558675433410252</v>
       </c>
       <c r="E6" s="14">
-        <f>E$68/E48</f>
-        <v>2.3313088981452279</v>
+        <f t="shared" si="0"/>
+        <v>3.8826195279579725</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -915,16 +1038,16 @@
         <v>8</v>
       </c>
       <c r="C7" s="12">
-        <f>C$68/C49</f>
-        <v>6.4772430586531149</v>
+        <f t="shared" si="0"/>
+        <v>2.6776708299405585</v>
       </c>
       <c r="D7" s="12">
-        <f>D$68/D49</f>
-        <v>6.5135114829797809</v>
+        <f t="shared" si="0"/>
+        <v>4.5437231070536752</v>
       </c>
       <c r="E7" s="14">
-        <f>E$68/E49</f>
-        <v>4.6447813944152392</v>
+        <f t="shared" si="0"/>
+        <v>5.0733815644863416</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1046,16 +1169,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="12">
-        <f t="shared" ref="C11:E11" si="0">C$69/C53</f>
-        <v>1.6815001341689693</v>
+        <f t="shared" ref="C11:E11" si="1">C$69/C53</f>
+        <v>6.6368388213580598E-2</v>
       </c>
       <c r="D11" s="12">
-        <f t="shared" si="0"/>
-        <v>1.5712029410811386</v>
+        <f t="shared" si="1"/>
+        <v>1.1449431280466043</v>
       </c>
       <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>1.6484792660309271</v>
+        <f t="shared" si="1"/>
+        <v>1.9535895009745703</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1085,16 +1208,16 @@
         <v>4</v>
       </c>
       <c r="C12" s="12">
-        <f t="shared" ref="C12:E12" si="1">C$69/C54</f>
-        <v>2.6855613653624038</v>
+        <f t="shared" ref="C12:E12" si="2">C$69/C54</f>
+        <v>2.8182396618142876E-2</v>
       </c>
       <c r="D12" s="12">
-        <f t="shared" si="1"/>
-        <v>3.0998482471871482</v>
+        <f t="shared" si="2"/>
+        <v>1.7392014927526571</v>
       </c>
       <c r="E12" s="14">
-        <f t="shared" si="1"/>
-        <v>3.3077887041513012</v>
+        <f t="shared" si="2"/>
+        <v>3.7113529557100682</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1124,16 +1247,16 @@
         <v>8</v>
       </c>
       <c r="C13" s="12">
-        <f t="shared" ref="C13:E13" si="2">C$69/C55</f>
-        <v>4.443964640306703</v>
+        <f t="shared" ref="C13:E13" si="3">C$69/C55</f>
+        <v>1.3633579707124498E-2</v>
       </c>
       <c r="D13" s="12">
-        <f t="shared" si="2"/>
-        <v>6.095078127857759</v>
+        <f t="shared" si="3"/>
+        <v>1.3301785699297586</v>
       </c>
       <c r="E13" s="14">
-        <f t="shared" si="2"/>
-        <v>6.6045696764667241</v>
+        <f t="shared" si="3"/>
+        <v>4.8203156788537456</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1257,16 +1380,16 @@
         <v>2</v>
       </c>
       <c r="C17" s="12">
-        <f t="shared" ref="C17:E17" si="3">C$70/C59</f>
-        <v>1.6618968110317904</v>
+        <f t="shared" ref="C17:E17" si="4">C$70/C59</f>
+        <v>1.7151741915978829</v>
       </c>
       <c r="D17" s="12">
-        <f t="shared" si="3"/>
-        <v>1.6466742003324515</v>
+        <f t="shared" si="4"/>
+        <v>1.9386388457087</v>
       </c>
       <c r="E17" s="13">
-        <f t="shared" si="3"/>
-        <v>1.613991002265839</v>
+        <f t="shared" si="4"/>
+        <v>1.9646197293613417</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1296,16 +1419,16 @@
         <v>4</v>
       </c>
       <c r="C18" s="12">
-        <f t="shared" ref="C18:E18" si="4">C$70/C60</f>
-        <v>3.2761118631397075</v>
+        <f t="shared" ref="C18:E18" si="5">C$70/C60</f>
+        <v>2.7677056166211029</v>
       </c>
       <c r="D18" s="12">
-        <f t="shared" si="4"/>
-        <v>3.3069757306377388</v>
+        <f t="shared" si="5"/>
+        <v>3.500487815244635</v>
       </c>
       <c r="E18" s="14">
-        <f t="shared" si="4"/>
-        <v>3.2422204473020262</v>
+        <f t="shared" si="5"/>
+        <v>3.0856594101887929</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1335,16 +1458,16 @@
         <v>8</v>
       </c>
       <c r="C19" s="12">
-        <f t="shared" ref="C19:E19" si="5">C$70/C61</f>
-        <v>6.3250585240766126</v>
+        <f t="shared" ref="C19:E19" si="6">C$70/C61</f>
+        <v>2.7913923612087372</v>
       </c>
       <c r="D19" s="12">
-        <f t="shared" si="5"/>
-        <v>6.6094088060739731</v>
+        <f t="shared" si="6"/>
+        <v>4.4816886811814998</v>
       </c>
       <c r="E19" s="14">
-        <f t="shared" si="5"/>
-        <v>6.4135569500361616</v>
+        <f t="shared" si="6"/>
+        <v>3.7258063130127095</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1516,14 +1639,14 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34">
+      <c r="B25" s="32"/>
+      <c r="C25" s="33">
         <v>5000</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="33">
         <v>50000</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="34">
         <v>500000</v>
       </c>
       <c r="F25" s="2"/>
@@ -1550,20 +1673,20 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="36">
+      <c r="B26" s="35">
         <v>2</v>
       </c>
-      <c r="C26" s="37">
-        <f t="shared" ref="C26:E26" si="6">C5/$B$26</f>
-        <v>0.82559187737245243</v>
+      <c r="C26" s="54">
+        <f t="shared" ref="C26:E26" si="7">C5/$B$26</f>
+        <v>0.74274051186662471</v>
       </c>
-      <c r="D26" s="37">
-        <f t="shared" si="6"/>
-        <v>0.67611214574102418</v>
+      <c r="D26" s="54">
+        <f t="shared" si="7"/>
+        <v>0.9719768012464689</v>
       </c>
-      <c r="E26" s="38">
-        <f t="shared" si="6"/>
-        <v>0.5616210777044407</v>
+      <c r="E26" s="55">
+        <f t="shared" si="7"/>
+        <v>0.99556457016703503</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1589,20 +1712,20 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="36">
+      <c r="B27" s="35">
         <v>4</v>
       </c>
-      <c r="C27" s="37">
-        <f t="shared" ref="C27:E27" si="7">C6/$B$27</f>
-        <v>0.81891642275970233</v>
+      <c r="C27" s="36">
+        <f t="shared" ref="C27:E27" si="8">C6/$B$27</f>
+        <v>0.65981260730105173</v>
       </c>
-      <c r="D27" s="37">
-        <f t="shared" si="7"/>
-        <v>0.82753185457332079</v>
+      <c r="D27" s="36">
+        <f t="shared" si="8"/>
+        <v>0.88896688583525629</v>
       </c>
-      <c r="E27" s="39">
-        <f t="shared" si="7"/>
-        <v>0.58282722453630698</v>
+      <c r="E27" s="37">
+        <f t="shared" si="8"/>
+        <v>0.97065488198949312</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1628,20 +1751,20 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
-      <c r="B28" s="36">
+      <c r="B28" s="35">
         <v>8</v>
       </c>
-      <c r="C28" s="37">
-        <f t="shared" ref="C28:E28" si="8">C7/$B$28</f>
-        <v>0.80965538233163936</v>
+      <c r="C28" s="36">
+        <f t="shared" ref="C28:E28" si="9">C7/$B$28</f>
+        <v>0.33470885374256981</v>
       </c>
-      <c r="D28" s="37">
-        <f t="shared" si="8"/>
-        <v>0.81418893537247261</v>
+      <c r="D28" s="36">
+        <f t="shared" si="9"/>
+        <v>0.5679653883817094</v>
       </c>
-      <c r="E28" s="39">
-        <f t="shared" si="8"/>
-        <v>0.5805976743019049</v>
+      <c r="E28" s="37">
+        <f t="shared" si="9"/>
+        <v>0.6341726955607927</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1667,10 +1790,10 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1695,12 +1818,12 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1725,14 +1848,14 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="34">
+      <c r="B31" s="32"/>
+      <c r="C31" s="33">
         <v>100</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="33">
         <v>1000</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="34">
         <v>10000</v>
       </c>
       <c r="F31" s="21"/>
@@ -1759,20 +1882,20 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="36">
+      <c r="B32" s="35">
         <v>2</v>
       </c>
-      <c r="C32" s="37">
-        <f t="shared" ref="C32:E32" si="9">C11/$B$26</f>
-        <v>0.84075006708448463</v>
+      <c r="C32" s="54">
+        <f t="shared" ref="C32:E32" si="10">C11/$B$26</f>
+        <v>3.3184194106790299E-2</v>
       </c>
-      <c r="D32" s="37">
-        <f t="shared" si="9"/>
-        <v>0.78560147054056928</v>
+      <c r="D32" s="54">
+        <f t="shared" si="10"/>
+        <v>0.57247156402330213</v>
       </c>
-      <c r="E32" s="38">
-        <f t="shared" si="9"/>
-        <v>0.82423963301546355</v>
+      <c r="E32" s="55">
+        <f t="shared" si="10"/>
+        <v>0.97679475048728515</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1798,20 +1921,20 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="36">
+      <c r="B33" s="35">
         <v>4</v>
       </c>
-      <c r="C33" s="37">
-        <f t="shared" ref="C33:E33" si="10">C12/$B$27</f>
-        <v>0.67139034134060094</v>
+      <c r="C33" s="36">
+        <f t="shared" ref="C33:E33" si="11">C12/$B$27</f>
+        <v>7.0455991545357189E-3</v>
       </c>
-      <c r="D33" s="37">
-        <f t="shared" si="10"/>
-        <v>0.77496206179678706</v>
+      <c r="D33" s="36">
+        <f t="shared" si="11"/>
+        <v>0.43480037318816428</v>
       </c>
-      <c r="E33" s="39">
-        <f t="shared" si="10"/>
-        <v>0.8269471760378253</v>
+      <c r="E33" s="37">
+        <f t="shared" si="11"/>
+        <v>0.92783823892751704</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1837,20 +1960,20 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="36">
+      <c r="B34" s="35">
         <v>8</v>
       </c>
-      <c r="C34" s="37">
-        <f t="shared" ref="C34:E34" si="11">C13/$B$28</f>
-        <v>0.55549558003833788</v>
+      <c r="C34" s="36">
+        <f t="shared" ref="C34:E34" si="12">C13/$B$28</f>
+        <v>1.7041974633905622E-3</v>
       </c>
-      <c r="D34" s="37">
-        <f t="shared" si="11"/>
-        <v>0.76188476598221988</v>
+      <c r="D34" s="36">
+        <f t="shared" si="12"/>
+        <v>0.16627232124121982</v>
       </c>
-      <c r="E34" s="39">
-        <f t="shared" si="11"/>
-        <v>0.82557120955834051</v>
+      <c r="E34" s="37">
+        <f t="shared" si="12"/>
+        <v>0.6025394598567182</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1876,10 +1999,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="1"/>
@@ -1904,14 +2027,14 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="46"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="1"/>
@@ -1936,14 +2059,14 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34">
+      <c r="B37" s="32"/>
+      <c r="C37" s="33">
         <v>5000</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="33">
         <v>50000</v>
       </c>
-      <c r="E37" s="35">
+      <c r="E37" s="34">
         <v>500000</v>
       </c>
       <c r="F37" s="21"/>
@@ -1970,20 +2093,20 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="36">
+      <c r="B38" s="35">
         <v>2</v>
       </c>
-      <c r="C38" s="37">
-        <f t="shared" ref="C38:E38" si="12">C17/$B$26</f>
-        <v>0.83094840551589522</v>
+      <c r="C38" s="54">
+        <f t="shared" ref="C38:E38" si="13">C17/$B$26</f>
+        <v>0.85758709579894143</v>
       </c>
-      <c r="D38" s="37">
-        <f t="shared" si="12"/>
-        <v>0.82333710016622574</v>
+      <c r="D38" s="54">
+        <f t="shared" si="13"/>
+        <v>0.96931942285435002</v>
       </c>
-      <c r="E38" s="38">
-        <f t="shared" si="12"/>
-        <v>0.80699550113291951</v>
+      <c r="E38" s="55">
+        <f t="shared" si="13"/>
+        <v>0.98230986468067083</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2009,20 +2132,20 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="36">
+      <c r="B39" s="35">
         <v>4</v>
       </c>
-      <c r="C39" s="37">
-        <f t="shared" ref="C39:E39" si="13">C18/$B$27</f>
-        <v>0.81902796578492687</v>
+      <c r="C39" s="36">
+        <f t="shared" ref="C39:E39" si="14">C18/$B$27</f>
+        <v>0.69192640415527573</v>
       </c>
-      <c r="D39" s="37">
-        <f t="shared" si="13"/>
-        <v>0.82674393265943469</v>
+      <c r="D39" s="36">
+        <f t="shared" si="14"/>
+        <v>0.87512195381115876</v>
       </c>
-      <c r="E39" s="39">
-        <f t="shared" si="13"/>
-        <v>0.81055511182550655</v>
+      <c r="E39" s="37">
+        <f t="shared" si="14"/>
+        <v>0.77141485254719822</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -2048,20 +2171,20 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="36">
+      <c r="B40" s="35">
         <v>8</v>
       </c>
-      <c r="C40" s="37">
-        <f t="shared" ref="C40:E40" si="14">C19/$B$28</f>
-        <v>0.79063231550957658</v>
+      <c r="C40" s="36">
+        <f t="shared" ref="C40:E40" si="15">C19/$B$28</f>
+        <v>0.34892404515109215</v>
       </c>
-      <c r="D40" s="37">
-        <f t="shared" si="14"/>
-        <v>0.82617610075924663</v>
+      <c r="D40" s="36">
+        <f t="shared" si="15"/>
+        <v>0.56021108514768747</v>
       </c>
-      <c r="E40" s="39">
-        <f t="shared" si="14"/>
-        <v>0.80169461875452019</v>
+      <c r="E40" s="37">
+        <f t="shared" si="15"/>
+        <v>0.46572578912658869</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -2087,10 +2210,10 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="41"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="1"/>
@@ -2273,13 +2396,13 @@
         <v>2</v>
       </c>
       <c r="C47" s="7">
-        <v>2.0385980606079102E-2</v>
+        <v>2.2660000002360899E-2</v>
       </c>
       <c r="D47" s="7">
-        <v>0.24911399841308501</v>
+        <v>0.17328499999712199</v>
       </c>
       <c r="E47" s="22">
-        <v>2.9898539543151799</v>
+        <v>1.68664599998737</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2309,13 +2432,13 @@
         <v>4</v>
       </c>
       <c r="C48" s="7">
-        <v>1.02760791778564E-2</v>
+        <v>1.27540000103181E-2</v>
       </c>
       <c r="D48" s="7">
-        <v>0.10176587104797299</v>
+        <v>9.4733000005362597E-2</v>
       </c>
       <c r="E48" s="22">
-        <v>1.44053411483764</v>
+        <v>0.86496500000066501</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2345,13 +2468,13 @@
         <v>8</v>
       </c>
       <c r="C49" s="7">
-        <v>5.1968097686768003E-3</v>
+        <v>1.25709999992978E-2</v>
       </c>
       <c r="D49" s="7">
-        <v>5.1716804504394497E-2</v>
+        <v>7.4137000003247494E-2</v>
       </c>
       <c r="E49" s="22">
-        <v>0.72303295135498002</v>
+        <v>0.66195100000186302</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2476,16 +2599,18 @@
       <c r="B53" s="11">
         <v>2</v>
       </c>
-      <c r="C53" s="7">
-        <v>5.2928924560499997E-5</v>
+      <c r="C53" s="53">
+        <v>1.3409999955911001E-3</v>
       </c>
-      <c r="D53" s="7">
-        <v>4.7409534454345998E-3</v>
+      <c r="D53" s="53">
+        <v>6.5060000051743996E-3</v>
       </c>
       <c r="E53" s="22">
-        <v>0.40960478782653797</v>
+        <v>0.34563300000445402</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -2512,14 +2637,14 @@
       <c r="B54" s="11">
         <v>4</v>
       </c>
-      <c r="C54" s="7">
-        <v>3.3140182495100003E-5</v>
+      <c r="C54" s="53">
+        <v>3.1579999922542001E-3</v>
       </c>
-      <c r="D54" s="7">
-        <v>2.4030208587645999E-3</v>
+      <c r="D54" s="53">
+        <v>4.2830000020330997E-3</v>
       </c>
       <c r="E54" s="22">
-        <v>0.20413184165954501</v>
+        <v>0.18193500000052101</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2548,14 +2673,14 @@
       <c r="B55" s="11">
         <v>8</v>
       </c>
-      <c r="C55" s="26">
-        <v>2.0027160644500001E-5</v>
+      <c r="C55" s="53">
+        <v>6.5279999980702996E-3</v>
       </c>
-      <c r="D55" s="7">
-        <v>1.2221336364746001E-3</v>
+      <c r="D55" s="53">
+        <v>5.6000000040513E-3</v>
       </c>
       <c r="E55" s="22">
-        <v>0.102236032485961</v>
+        <v>0.14007900000433399</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2680,14 +2805,14 @@
       <c r="B59" s="11">
         <v>2</v>
       </c>
-      <c r="C59" s="7">
-        <v>2.04110145568848E-2</v>
+      <c r="C59" s="53">
+        <v>1.97770000086166E-2</v>
       </c>
-      <c r="D59" s="22">
-        <v>0.204815864562988</v>
+      <c r="D59" s="47">
+        <v>0.17397000000346399</v>
       </c>
-      <c r="E59" s="22">
-        <v>2.1490819931030201</v>
+      <c r="E59" s="50">
+        <v>1.7655319999903401</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2716,14 +2841,14 @@
       <c r="B60" s="11">
         <v>4</v>
       </c>
-      <c r="C60" s="7">
-        <v>1.03540420532227E-2</v>
+      <c r="C60" s="53">
+        <v>1.22559999872465E-2</v>
       </c>
-      <c r="D60" s="22">
-        <v>0.101985931396484</v>
+      <c r="D60" s="48">
+        <v>9.6347999991849106E-2</v>
       </c>
-      <c r="E60" s="22">
-        <v>1.0698220729827801</v>
+      <c r="E60" s="51">
+        <v>1.1241030000091901</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2752,14 +2877,14 @@
       <c r="B61" s="11">
         <v>8</v>
       </c>
-      <c r="C61" s="7">
-        <v>5.3629543304443E-3</v>
+      <c r="C61" s="53">
+        <v>1.2152000010246401E-2</v>
       </c>
-      <c r="D61" s="22">
-        <v>5.1028013229370103E-2</v>
+      <c r="D61" s="48">
+        <v>7.5253999995766194E-2</v>
       </c>
-      <c r="E61" s="22">
-        <v>0.54082298278808505</v>
+      <c r="E61" s="51">
+        <v>0.93096599999989804</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2787,8 +2912,8 @@
       <c r="A62" s="1"/>
       <c r="B62" s="15"/>
       <c r="C62" s="24"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="52"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -2814,7 +2939,9 @@
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
@@ -2926,8 +3053,8 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="27"/>
-      <c r="B67" s="28" t="s">
+      <c r="A67" s="26"/>
+      <c r="B67" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C67" s="9">
@@ -2939,31 +3066,31 @@
       <c r="E67" s="10">
         <v>500000</v>
       </c>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="27"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="27"/>
-      <c r="P67" s="27"/>
-      <c r="Q67" s="27"/>
-      <c r="R67" s="27"/>
-      <c r="S67" s="27"/>
-      <c r="T67" s="27"/>
-      <c r="U67" s="27"/>
-      <c r="V67" s="27"/>
-      <c r="W67" s="27"/>
-      <c r="X67" s="27"/>
-      <c r="Y67" s="27"/>
-      <c r="Z67" s="27"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="26"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="26"/>
+      <c r="N67" s="26"/>
+      <c r="O67" s="26"/>
+      <c r="P67" s="26"/>
+      <c r="Q67" s="26"/>
+      <c r="R67" s="26"/>
+      <c r="S67" s="26"/>
+      <c r="T67" s="26"/>
+      <c r="U67" s="26"/>
+      <c r="V67" s="26"/>
+      <c r="W67" s="26"/>
+      <c r="X67" s="26"/>
+      <c r="Y67" s="26"/>
+      <c r="Z67" s="26"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
-      <c r="B68" s="29" t="s">
+      <c r="B68" s="28" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="24">
@@ -2999,11 +3126,11 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="24">
-        <v>8.8999993749900002E-5</v>
+        <v>8.9000008301799998E-5</v>
       </c>
       <c r="D69" s="24">
         <v>7.4489999969956002E-3</v>
@@ -3041,16 +3168,16 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="48">
+      <c r="C70" s="46">
         <v>3.3921000002010301E-2</v>
       </c>
       <c r="D70" s="24">
         <v>0.33726499999465798</v>
       </c>
-      <c r="E70" s="30">
+      <c r="E70" s="29">
         <v>3.4685989999998101</v>
       </c>
       <c r="F70" s="5"/>
@@ -3076,32 +3203,32 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="31"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="31"/>
-      <c r="P71" s="31"/>
-      <c r="Q71" s="31"/>
-      <c r="R71" s="31"/>
-      <c r="S71" s="31"/>
-      <c r="T71" s="31"/>
-      <c r="U71" s="31"/>
-      <c r="V71" s="31"/>
-      <c r="W71" s="31"/>
-      <c r="X71" s="31"/>
-      <c r="Y71" s="31"/>
-      <c r="Z71" s="31"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="30"/>
+      <c r="J71" s="30"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="30"/>
+      <c r="M71" s="30"/>
+      <c r="N71" s="30"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30"/>
+      <c r="Q71" s="30"/>
+      <c r="R71" s="30"/>
+      <c r="S71" s="30"/>
+      <c r="T71" s="30"/>
+      <c r="U71" s="30"/>
+      <c r="V71" s="30"/>
+      <c r="W71" s="30"/>
+      <c r="X71" s="30"/>
+      <c r="Y71" s="30"/>
+      <c r="Z71" s="30"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
@@ -3140,11 +3267,11 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="32"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31"/>
+      <c r="M73" s="31"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -3168,11 +3295,11 @@
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="32"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+      <c r="M74" s="31"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
@@ -3198,11 +3325,11 @@
         <v>8</v>
       </c>
       <c r="H75" s="1"/>
-      <c r="I75" s="32"/>
-      <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
-      <c r="L75" s="32"/>
-      <c r="M75" s="32"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
@@ -3226,11 +3353,11 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="32"/>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-      <c r="M76" s="32"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="31"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>

</xml_diff>